<commit_message>
add clip_flood_data, add 'if damage.empty'
</commit_message>
<xml_diff>
--- a/output/damage/TWN_osm_fl_historical_damage_1.xlsx
+++ b/output/damage/TWN_osm_fl_historical_damage_1.xlsx
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1658665304.414537</v>
+        <v>1676554327.812017</v>
       </c>
       <c r="F2" t="n">
-        <v>452363264.8403282</v>
+        <v>457242089.4032773</v>
       </c>
       <c r="G2" t="n">
-        <v>2261816324.201641</v>
+        <v>2286210447.016387</v>
       </c>
     </row>
     <row r="3">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4614857.165971609</v>
+        <v>4874074.231378612</v>
       </c>
       <c r="F3" t="n">
-        <v>1730571.437239354</v>
+        <v>1827777.83676698</v>
       </c>
       <c r="G3" t="n">
-        <v>8652857.186196769</v>
+        <v>9138889.183834899</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1730780851.576564</v>
+        <v>1748273275.282674</v>
       </c>
       <c r="F4" t="n">
-        <v>472031141.3390628</v>
+        <v>476801802.3498201</v>
       </c>
       <c r="G4" t="n">
-        <v>2360155706.695314</v>
+        <v>2384009011.7491</v>
       </c>
     </row>
     <row r="5">
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4703594.243019414</v>
+        <v>4962811.308426417</v>
       </c>
       <c r="F5" t="n">
-        <v>1763847.841132281</v>
+        <v>1861054.240659907</v>
       </c>
       <c r="G5" t="n">
-        <v>8819239.205661405</v>
+        <v>9305271.203299535</v>
       </c>
     </row>
     <row r="6">
@@ -601,13 +601,13 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2388257751.201511</v>
+        <v>2389772841.46038</v>
       </c>
       <c r="F6" t="n">
-        <v>651343023.0549576</v>
+        <v>651756229.4891943</v>
       </c>
       <c r="G6" t="n">
-        <v>3256715115.274788</v>
+        <v>3258781147.445971</v>
       </c>
     </row>
     <row r="7">
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6540314.578311968</v>
+        <v>6697133.033314341</v>
       </c>
       <c r="F7" t="n">
-        <v>2452617.966866988</v>
+        <v>2511424.887492878</v>
       </c>
       <c r="G7" t="n">
-        <v>12263089.83433494</v>
+        <v>12557124.43746439</v>
       </c>
     </row>
     <row r="8">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2552940283.884904</v>
+        <v>2554361971.929386</v>
       </c>
       <c r="F8" t="n">
-        <v>696256441.0595193</v>
+        <v>696644174.1625597</v>
       </c>
       <c r="G8" t="n">
-        <v>3481282205.297596</v>
+        <v>3483220870.812799</v>
       </c>
     </row>
     <row r="9">
@@ -688,13 +688,13 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>6904517.656745113</v>
+        <v>7061336.111747485</v>
       </c>
       <c r="F9" t="n">
-        <v>2589194.121279418</v>
+        <v>2648001.041905307</v>
       </c>
       <c r="G9" t="n">
-        <v>12945970.60639709</v>
+        <v>13240005.20952654</v>
       </c>
     </row>
     <row r="10">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2767453831.218783</v>
+        <v>2768713698.614011</v>
       </c>
       <c r="F10" t="n">
-        <v>754760135.7869407</v>
+        <v>755103735.9856393</v>
       </c>
       <c r="G10" t="n">
-        <v>3773800678.934703</v>
+        <v>3775518679.928197</v>
       </c>
     </row>
     <row r="11">
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7130536.56873311</v>
+        <v>7287355.023735483</v>
       </c>
       <c r="F11" t="n">
-        <v>2673951.213274917</v>
+        <v>2732758.133900806</v>
       </c>
       <c r="G11" t="n">
-        <v>13369756.06637458</v>
+        <v>13663790.66950403</v>
       </c>
     </row>
     <row r="12">
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2921201118.422153</v>
+        <v>2922421891.706268</v>
       </c>
       <c r="F12" t="n">
-        <v>796691214.1151325</v>
+        <v>797024152.2835275</v>
       </c>
       <c r="G12" t="n">
-        <v>3983456070.575663</v>
+        <v>3985120761.417638</v>
       </c>
     </row>
     <row r="13">
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>7199424.826596685</v>
+        <v>7356243.281599058</v>
       </c>
       <c r="F13" t="n">
-        <v>2699784.309973757</v>
+        <v>2758591.230599647</v>
       </c>
       <c r="G13" t="n">
-        <v>13498921.54986879</v>
+        <v>13792956.15299824</v>
       </c>
     </row>
     <row r="14">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3080762155.186232</v>
+        <v>3081982928.470347</v>
       </c>
       <c r="F14" t="n">
-        <v>840207860.5053358</v>
+        <v>840540798.6737309</v>
       </c>
       <c r="G14" t="n">
-        <v>4201039302.526679</v>
+        <v>4202703993.368654</v>
       </c>
     </row>
     <row r="15">
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>7337966.279859954</v>
+        <v>7444045.18904587</v>
       </c>
       <c r="F15" t="n">
-        <v>2751737.354947484</v>
+        <v>2791516.945892202</v>
       </c>
       <c r="G15" t="n">
-        <v>13758686.77473742</v>
+        <v>13957584.72946101</v>
       </c>
     </row>
     <row r="16">
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3356950492.107258</v>
+        <v>3357934556.155107</v>
       </c>
       <c r="F16" t="n">
-        <v>915531952.3928884</v>
+        <v>915800333.4968474</v>
       </c>
       <c r="G16" t="n">
-        <v>4577659761.964442</v>
+        <v>4579001667.484237</v>
       </c>
     </row>
     <row r="17">
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>7585611.486911032</v>
+        <v>7640031.331508775</v>
       </c>
       <c r="F17" t="n">
-        <v>2844604.307591638</v>
+        <v>2865011.749315791</v>
       </c>
       <c r="G17" t="n">
-        <v>14223021.53795819</v>
+        <v>14325058.74657895</v>
       </c>
     </row>
     <row r="18">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>7795778.613512935</v>
+        <v>7809483.843159612</v>
       </c>
       <c r="F19" t="n">
-        <v>2923416.980067351</v>
+        <v>2928556.441184855</v>
       </c>
       <c r="G19" t="n">
-        <v>14617084.90033675</v>
+        <v>14642782.20592427</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
add lower/upper risk, and set ne_path
</commit_message>
<xml_diff>
--- a/output/damage/TWN_osm_fl_historical_damage_1.xlsx
+++ b/output/damage/TWN_osm_fl_historical_damage_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,365 +449,600 @@
           <t>asset_type</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>meandam</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>lowerdam</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>upperdam</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>rp0001</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>544840920.5143894</v>
+      </c>
+      <c r="F2" t="n">
+        <v>408630690.385792</v>
+      </c>
+      <c r="G2" t="n">
+        <v>681051150.6429868</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>rp0001</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E3" t="n">
+        <v>5989529.050910485</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4492146.788182863</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7486911.313638107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.5</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>rp0002</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E4" t="n">
+        <v>568529545.9378448</v>
+      </c>
+      <c r="F4" t="n">
+        <v>426397159.4533835</v>
+      </c>
+      <c r="G4" t="n">
+        <v>710661932.4223059</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.5</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>rp0002</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E5" t="n">
+        <v>6104699.094479713</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4578524.320859784</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7630873.868099641</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.2</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>rp0005</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E6" t="n">
+        <v>784498565.2783953</v>
+      </c>
+      <c r="F6" t="n">
+        <v>588373923.9587964</v>
+      </c>
+      <c r="G6" t="n">
+        <v>980623206.5979941</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.2</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>rp0005</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8488540.979717484</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6366405.734788112</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10610676.22464686</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.1</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E8" t="n">
+        <v>838593735.9322069</v>
+      </c>
+      <c r="F8" t="n">
+        <v>628945301.9491551</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1048242169.915259</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.1</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8961232.731651062</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6720924.548738295</v>
+      </c>
+      <c r="G9" t="n">
+        <v>11201540.91456383</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.04</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E10" t="n">
+        <v>909057474.6268866</v>
+      </c>
+      <c r="F10" t="n">
+        <v>681793105.9701649</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1136321843.283608</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.04</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E11" t="n">
+        <v>9254578.070568452</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6940933.552926338</v>
+      </c>
+      <c r="G11" t="n">
+        <v>11568222.58821057</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>0.02</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E12" t="n">
+        <v>959560619.0910087</v>
+      </c>
+      <c r="F12" t="n">
+        <v>719670464.3182564</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1199450773.863761</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
-        <v>0.02</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E13" t="n">
+        <v>9343986.736297682</v>
+      </c>
+      <c r="F13" t="n">
+        <v>7007990.052223261</v>
+      </c>
+      <c r="G13" t="n">
+        <v>11679983.4203721</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
-        <v>0.01</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1011973472.918356</v>
+      </c>
+      <c r="F14" t="n">
+        <v>758980104.6887666</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1264966841.147944</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
-        <v>0.01</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E15" t="n">
+        <v>9523796.864592521</v>
+      </c>
+      <c r="F15" t="n">
+        <v>7142847.64844439</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11904746.08074065</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
-        <v>0.004</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1102696240.991511</v>
+      </c>
+      <c r="F16" t="n">
+        <v>827022180.7436334</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1378370301.239389</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
-        <v>0.004</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E17" t="n">
+        <v>9845210.531062711</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7383907.898297034</v>
+      </c>
+      <c r="G17" t="n">
+        <v>12306513.16382839</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
-        <v>0.002</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1159107516.433252</v>
+      </c>
+      <c r="F18" t="n">
+        <v>869330637.3249388</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1448884395.541565</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
-        <v>0.002</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E19" t="n">
+        <v>10117982.16083502</v>
+      </c>
+      <c r="F19" t="n">
+        <v>7588486.620626263</v>
+      </c>
+      <c r="G19" t="n">
+        <v>12647477.70104377</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
-        <v>0.001</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>F1_1</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>plant</t>
         </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1214875594.003349</v>
+      </c>
+      <c r="F20" t="n">
+        <v>911156695.5025115</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1518594492.504186</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
-        <v>0.001</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>F2_1</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>substation</t>
         </is>
+      </c>
+      <c r="E21" t="n">
+        <v>10494878.79046413</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7871159.092848093</v>
+      </c>
+      <c r="G21" t="n">
+        <v>13118598.48808016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>